<commit_message>
Add placeholders for hosuing 2 charts, update docs
</commit_message>
<xml_diff>
--- a/docs/housing_story_content/housing data story.xlsx
+++ b/docs/housing_story_content/housing data story.xlsx
@@ -9,19 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" firstSheet="3" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="(1) population &amp; households" sheetId="1" r:id="rId1"/>
     <sheet name="(2) type of housing" sheetId="2" r:id="rId2"/>
     <sheet name="(3) housing completions" sheetId="3" r:id="rId3"/>
-    <sheet name="(4) social housing completions" sheetId="4" r:id="rId4"/>
-    <sheet name="(5) house prices" sheetId="5" r:id="rId5"/>
-    <sheet name="(6) property price index" sheetId="13" r:id="rId6"/>
-    <sheet name="(7) rent" sheetId="26" r:id="rId7"/>
-    <sheet name="(8) mortgages arrears" sheetId="7" r:id="rId8"/>
-    <sheet name="(9) BTL arrears" sheetId="8" r:id="rId9"/>
-    <sheet name="Charts In Use" sheetId="32" r:id="rId10"/>
+    <sheet name="Charts In Use" sheetId="32" r:id="rId4"/>
+    <sheet name="(4) social housing completions" sheetId="4" r:id="rId5"/>
+    <sheet name="(5) house prices" sheetId="5" r:id="rId6"/>
+    <sheet name="(6) property price index" sheetId="13" r:id="rId7"/>
+    <sheet name="(7) rent" sheetId="26" r:id="rId8"/>
+    <sheet name="(8) mortgages arrears" sheetId="7" r:id="rId9"/>
+    <sheet name="(9) BTL arrears" sheetId="8" r:id="rId10"/>
     <sheet name="(10) residential mortgage debt" sheetId="9" r:id="rId11"/>
     <sheet name="(11) traveller accommodation" sheetId="10" r:id="rId12"/>
     <sheet name="(12) serviced zoned land" sheetId="11" r:id="rId13"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1862" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1889" uniqueCount="568">
   <si>
     <t>Fingal</t>
   </si>
@@ -1623,9 +1623,6 @@
     <t>The new data csv to be used</t>
   </si>
   <si>
-    <t>PHASE 2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Location </t>
   </si>
   <si>
@@ -1677,13 +1674,144 @@
     <t>#serviced-land-expected-units-chart</t>
   </si>
   <si>
-    <t>#negative-equity-chart?</t>
-  </si>
-  <si>
     <t>Home mortgage arrears graph (total, total over 90 days &amp; % over 90 days)</t>
   </si>
   <si>
     <t>#home-mortgage-arrears-chart</t>
+  </si>
+  <si>
+    <r>
+      <t>Buy-to-let</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>mortgage arrears graph (total, total over 90 days &amp; % over 90 days)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Vacant housing 1991-2016 [line graph] – nationwide (one tab – needs numbers and %) and 4 Dublin LAs and Meath, Kildare and Wicklow (another tab)  </t>
+  </si>
+  <si>
+    <r>
+      <t>Tab 17,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CSO various censuses</t>
+    </r>
+  </si>
+  <si>
+    <t>Map of unfinished estates in four Dublin LAs, and Meath, Kildare and Wicklow in 2010 &amp; 2017</t>
+  </si>
+  <si>
+    <t>Needs proportional circle to represent number of units in each estate.</t>
+  </si>
+  <si>
+    <t>Data in two excel separate files</t>
+  </si>
+  <si>
+    <t>Data provided</t>
+  </si>
+  <si>
+    <t>Time-seried graph of serviced and unserviced zone land in four Dublin LAs, and Meath, Kildare and Wicklow in 2008</t>
+  </si>
+  <si>
+    <t>Entry</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Tab 12, DEHLG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Map of zoned areas in Dublin </t>
+  </si>
+  <si>
+    <t>AIRO</t>
+  </si>
+  <si>
+    <t>#zoned-areas-map</t>
+  </si>
+  <si>
+    <t>Home mortgage arrears</t>
+  </si>
+  <si>
+    <t>Tab 8 – Central Bank</t>
+  </si>
+  <si>
+    <t>Buy-to-let mortgage arrears</t>
+  </si>
+  <si>
+    <t>Social housing waiting list data 1991-present</t>
+  </si>
+  <si>
+    <t>Tab 14 - DECLG</t>
+  </si>
+  <si>
+    <t>Rent supplement figures – numbers and costs</t>
+  </si>
+  <si>
+    <t>Need to find source – probably https://www.welfare.ie/en/Pages/Annual-SWS-Statistical-Information-Report.aspx</t>
+  </si>
+  <si>
+    <t>Figures relating to different PPP schemes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tab 20 - Spatial justice chapter  </t>
+  </si>
+  <si>
+    <t>Traveller accommodation figures</t>
+  </si>
+  <si>
+    <t>Tab 11 - DECLG</t>
+  </si>
+  <si>
+    <t>#social-housing-wait-chart</t>
+  </si>
+  <si>
+    <t>#rent-suppliment-chart</t>
+  </si>
+  <si>
+    <t>#ppp-schemes-chart</t>
+  </si>
+  <si>
+    <t>#traveller-accomodation-chart</t>
   </si>
 </sst>
 </file>
@@ -1702,7 +1830,7 @@
     <numFmt numFmtId="171" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;?_-;_-@_-"/>
     <numFmt numFmtId="172" formatCode="0.0"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1860,6 +1988,38 @@
     <font>
       <i/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -3305,7 +3465,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3598,13 +3758,49 @@
     <xf numFmtId="3" fontId="14" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="728" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="728" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="733">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -4490,8 +4686,8 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="-1712446368"/>
-        <c:axId val="-1712443888"/>
+        <c:axId val="-1848856448"/>
+        <c:axId val="-1848854128"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -4567,11 +4763,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1712440896"/>
-        <c:axId val="-1712438416"/>
+        <c:axId val="-1848851296"/>
+        <c:axId val="-1848848976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1712446368"/>
+        <c:axId val="-1848856448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4598,7 +4794,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1712443888"/>
+        <c:crossAx val="-1848854128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4606,7 +4802,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1712443888"/>
+        <c:axId val="-1848854128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="8500.0"/>
@@ -4641,12 +4837,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1712446368"/>
+        <c:crossAx val="-1848856448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-1712440896"/>
+        <c:axId val="-1848851296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4655,7 +4851,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1712438416"/>
+        <c:crossAx val="-1848848976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4663,7 +4859,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1712438416"/>
+        <c:axId val="-1848848976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="18.0"/>
@@ -4692,7 +4888,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1712440896"/>
+        <c:crossAx val="-1848851296"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4746,7 +4942,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4790,7 +4986,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4834,7 +5030,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4878,7 +5074,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4922,7 +5118,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4971,7 +5167,7 @@
         <xdr:cNvPr id="2" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1500-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6520,125 +6716,586 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="C1:AN20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.33203125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="22.5" style="6" customWidth="1"/>
-    <col min="3" max="3" width="20.5" style="6" customWidth="1"/>
-    <col min="4" max="4" width="38.1640625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="45" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="6"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="28" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B1" s="6" t="s">
-        <v>521</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>522</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>523</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>524</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>525</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>527</v>
-      </c>
-      <c r="D5" s="148" t="s">
-        <v>529</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>530</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>531</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A10" s="149" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A11" s="150" t="s">
-        <v>89</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A12" s="149" t="s">
-        <v>90</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="A14" s="149" t="s">
-        <v>539</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>540</v>
-      </c>
-      <c r="D14" s="148" t="s">
+    <row r="1" spans="3:29" x14ac:dyDescent="0.2">
+      <c r="C1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" t="s">
+        <v>507</v>
+      </c>
+      <c r="G1" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="2" spans="3:29" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="3:29" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="B16" s="6" t="s">
-        <v>534</v>
-      </c>
-      <c r="D16" s="148" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" s="6" t="s">
-        <v>538</v>
-      </c>
+    <row r="6" spans="3:29" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="3:29" x14ac:dyDescent="0.2">
+      <c r="E7" s="24">
+        <v>41089</v>
+      </c>
+      <c r="F7" s="24">
+        <v>41180</v>
+      </c>
+      <c r="G7" s="24">
+        <v>41274</v>
+      </c>
+      <c r="H7" s="24">
+        <v>41361</v>
+      </c>
+      <c r="I7" s="24">
+        <v>41453</v>
+      </c>
+      <c r="J7" s="24">
+        <v>41547</v>
+      </c>
+      <c r="K7" s="24">
+        <v>41639</v>
+      </c>
+      <c r="L7" s="24">
+        <v>41729</v>
+      </c>
+      <c r="M7" s="24">
+        <v>41820</v>
+      </c>
+      <c r="N7" s="24">
+        <v>41912</v>
+      </c>
+      <c r="O7" s="24">
+        <v>42004</v>
+      </c>
+      <c r="P7" s="24">
+        <v>42094</v>
+      </c>
+      <c r="Q7" s="24">
+        <v>42185</v>
+      </c>
+      <c r="R7" s="24">
+        <v>42277</v>
+      </c>
+      <c r="S7" s="24">
+        <v>42369</v>
+      </c>
+      <c r="T7" s="24">
+        <v>42460</v>
+      </c>
+      <c r="U7" s="24">
+        <v>42551</v>
+      </c>
+      <c r="V7" s="24">
+        <v>42643</v>
+      </c>
+      <c r="W7" s="24">
+        <v>42734</v>
+      </c>
+      <c r="X7" s="24">
+        <v>42825</v>
+      </c>
+      <c r="Y7" s="24">
+        <v>42916</v>
+      </c>
+      <c r="Z7" s="24">
+        <v>43007</v>
+      </c>
+      <c r="AA7" s="24">
+        <v>43098</v>
+      </c>
+      <c r="AB7" s="24">
+        <v>43188</v>
+      </c>
+      <c r="AC7" s="90">
+        <v>43280</v>
+      </c>
+    </row>
+    <row r="8" spans="3:29" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I8" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" t="s">
+        <v>56</v>
+      </c>
+      <c r="K8" t="s">
+        <v>56</v>
+      </c>
+      <c r="L8" t="s">
+        <v>56</v>
+      </c>
+      <c r="M8" t="s">
+        <v>56</v>
+      </c>
+      <c r="N8" t="s">
+        <v>56</v>
+      </c>
+      <c r="O8" t="s">
+        <v>56</v>
+      </c>
+      <c r="P8" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>56</v>
+      </c>
+      <c r="R8" t="s">
+        <v>56</v>
+      </c>
+      <c r="S8" t="s">
+        <v>56</v>
+      </c>
+      <c r="T8" t="s">
+        <v>56</v>
+      </c>
+      <c r="U8" t="s">
+        <v>56</v>
+      </c>
+      <c r="V8" t="s">
+        <v>56</v>
+      </c>
+      <c r="W8" t="s">
+        <v>56</v>
+      </c>
+      <c r="X8" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="3:29" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="10" spans="3:29" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>289</v>
+      </c>
+      <c r="E10">
+        <v>150187</v>
+      </c>
+      <c r="F10">
+        <v>150544</v>
+      </c>
+      <c r="G10">
+        <v>150124</v>
+      </c>
+      <c r="H10">
+        <v>149395</v>
+      </c>
+      <c r="I10">
+        <v>148529</v>
+      </c>
+      <c r="J10">
+        <v>147610</v>
+      </c>
+      <c r="K10">
+        <v>145528</v>
+      </c>
+      <c r="L10">
+        <v>144686</v>
+      </c>
+      <c r="M10">
+        <v>144187</v>
+      </c>
+      <c r="N10">
+        <v>143354</v>
+      </c>
+      <c r="O10">
+        <v>140995</v>
+      </c>
+      <c r="P10">
+        <v>139206</v>
+      </c>
+      <c r="Q10">
+        <v>137303</v>
+      </c>
+      <c r="R10">
+        <v>137805</v>
+      </c>
+      <c r="S10">
+        <v>137504</v>
+      </c>
+      <c r="T10">
+        <v>137239</v>
+      </c>
+      <c r="U10">
+        <v>135874</v>
+      </c>
+      <c r="V10">
+        <v>133401</v>
+      </c>
+      <c r="W10">
+        <v>131501</v>
+      </c>
+      <c r="X10">
+        <v>128899</v>
+      </c>
+      <c r="Y10">
+        <v>127704</v>
+      </c>
+      <c r="Z10">
+        <v>125381</v>
+      </c>
+      <c r="AA10">
+        <v>123269</v>
+      </c>
+      <c r="AB10">
+        <v>121029</v>
+      </c>
+      <c r="AC10">
+        <v>118234</v>
+      </c>
+    </row>
+    <row r="11" spans="3:29" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" t="s">
+        <v>371</v>
+      </c>
+      <c r="E11">
+        <v>34719</v>
+      </c>
+      <c r="F11">
+        <v>36635</v>
+      </c>
+      <c r="G11">
+        <v>37878</v>
+      </c>
+      <c r="H11">
+        <v>39371</v>
+      </c>
+      <c r="I11">
+        <v>39948</v>
+      </c>
+      <c r="J11">
+        <v>40396</v>
+      </c>
+      <c r="K11">
+        <v>39250</v>
+      </c>
+      <c r="L11">
+        <v>39361</v>
+      </c>
+      <c r="M11">
+        <v>39669</v>
+      </c>
+      <c r="N11">
+        <v>38463</v>
+      </c>
+      <c r="O11">
+        <v>35583</v>
+      </c>
+      <c r="P11">
+        <v>33475</v>
+      </c>
+      <c r="Q11">
+        <v>31524</v>
+      </c>
+      <c r="R11">
+        <v>30212</v>
+      </c>
+      <c r="S11">
+        <v>28760</v>
+      </c>
+      <c r="T11">
+        <v>28716</v>
+      </c>
+      <c r="U11">
+        <v>27793</v>
+      </c>
+      <c r="V11">
+        <v>26737</v>
+      </c>
+      <c r="W11">
+        <v>25871</v>
+      </c>
+      <c r="X11">
+        <v>25175</v>
+      </c>
+      <c r="Y11">
+        <v>24450</v>
+      </c>
+      <c r="Z11">
+        <v>23779</v>
+      </c>
+      <c r="AA11">
+        <v>23282</v>
+      </c>
+      <c r="AB11">
+        <v>22545</v>
+      </c>
+      <c r="AC11" s="91">
+        <v>21317</v>
+      </c>
+    </row>
+    <row r="12" spans="3:29" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12">
+        <v>24879</v>
+      </c>
+      <c r="F12">
+        <v>27018</v>
+      </c>
+      <c r="G12">
+        <v>28366</v>
+      </c>
+      <c r="H12">
+        <v>29369</v>
+      </c>
+      <c r="I12">
+        <v>30326</v>
+      </c>
+      <c r="J12">
+        <v>31178</v>
+      </c>
+      <c r="K12">
+        <v>30706</v>
+      </c>
+      <c r="L12">
+        <v>31048</v>
+      </c>
+      <c r="M12">
+        <v>31749</v>
+      </c>
+      <c r="N12">
+        <v>31619</v>
+      </c>
+      <c r="O12">
+        <v>29224</v>
+      </c>
+      <c r="P12">
+        <v>27492</v>
+      </c>
+      <c r="Q12">
+        <v>26071</v>
+      </c>
+      <c r="R12">
+        <v>24809</v>
+      </c>
+      <c r="S12">
+        <v>23344</v>
+      </c>
+      <c r="T12">
+        <v>23270</v>
+      </c>
+      <c r="U12">
+        <v>22666</v>
+      </c>
+      <c r="V12">
+        <v>22095</v>
+      </c>
+      <c r="W12">
+        <v>21113</v>
+      </c>
+      <c r="X12">
+        <v>20601</v>
+      </c>
+      <c r="Y12">
+        <v>20191</v>
+      </c>
+      <c r="Z12">
+        <v>19405</v>
+      </c>
+      <c r="AA12">
+        <v>19018</v>
+      </c>
+      <c r="AB12">
+        <v>18363</v>
+      </c>
+      <c r="AC12">
+        <v>17394</v>
+      </c>
+    </row>
+    <row r="13" spans="3:29" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="F13">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="G13">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="H13">
+        <v>19.7</v>
+      </c>
+      <c r="I13">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="J13">
+        <v>21.1</v>
+      </c>
+      <c r="K13">
+        <v>21.1</v>
+      </c>
+      <c r="L13">
+        <v>21.5</v>
+      </c>
+      <c r="M13">
+        <v>22</v>
+      </c>
+      <c r="N13">
+        <v>22.1</v>
+      </c>
+      <c r="O13">
+        <v>20.7</v>
+      </c>
+      <c r="P13">
+        <v>19.7</v>
+      </c>
+      <c r="Q13">
+        <v>19</v>
+      </c>
+      <c r="R13">
+        <v>18</v>
+      </c>
+      <c r="S13">
+        <v>17</v>
+      </c>
+      <c r="T13">
+        <v>17</v>
+      </c>
+      <c r="U13">
+        <v>16.7</v>
+      </c>
+      <c r="V13">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="W13">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="X13">
+        <v>16</v>
+      </c>
+      <c r="Y13">
+        <v>15.8</v>
+      </c>
+      <c r="Z13">
+        <v>15.5</v>
+      </c>
+      <c r="AA13">
+        <v>15.4</v>
+      </c>
+      <c r="AB13">
+        <v>15.2</v>
+      </c>
+      <c r="AC13">
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="20" spans="4:40" x14ac:dyDescent="0.2">
+      <c r="D20" s="25"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="26"/>
+      <c r="N20" s="27"/>
+      <c r="O20" s="26"/>
+      <c r="P20" s="27"/>
+      <c r="Q20" s="26"/>
+      <c r="R20" s="27"/>
+      <c r="S20" s="26"/>
+      <c r="T20" s="27"/>
+      <c r="U20" s="26"/>
+      <c r="V20" s="27"/>
+      <c r="W20" s="26"/>
+      <c r="X20" s="27"/>
+      <c r="Y20" s="26"/>
+      <c r="Z20" s="27"/>
+      <c r="AA20" s="26"/>
+      <c r="AB20" s="27"/>
+      <c r="AC20" s="26"/>
+      <c r="AD20" s="27"/>
+      <c r="AE20" s="26"/>
+      <c r="AF20" s="27"/>
+      <c r="AG20" s="26"/>
+      <c r="AH20" s="27"/>
+      <c r="AI20" s="26"/>
+      <c r="AJ20" s="27"/>
+      <c r="AK20" s="26"/>
+      <c r="AL20" s="27"/>
+      <c r="AM20" s="26"/>
+      <c r="AN20" s="31"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1"/>
-    <hyperlink ref="D14" r:id="rId2"/>
-    <hyperlink ref="D16" r:id="rId3"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -35445,6 +36102,219 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="43.5" style="154" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" style="154" customWidth="1"/>
+    <col min="3" max="4" width="22.5" style="154" customWidth="1"/>
+    <col min="5" max="5" width="20.5" style="154" customWidth="1"/>
+    <col min="6" max="6" width="38.1640625" style="154" customWidth="1"/>
+    <col min="7" max="7" width="45" style="154" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="154"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="162" t="s">
+        <v>547</v>
+      </c>
+      <c r="B1" s="162" t="s">
+        <v>548</v>
+      </c>
+      <c r="C1" s="162" t="s">
+        <v>520</v>
+      </c>
+      <c r="D1" s="162" t="s">
+        <v>545</v>
+      </c>
+      <c r="E1" s="162" t="s">
+        <v>521</v>
+      </c>
+      <c r="F1" s="162" t="s">
+        <v>522</v>
+      </c>
+      <c r="G1" s="154" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="B2" s="154" t="s">
+        <v>523</v>
+      </c>
+      <c r="C2" s="154" t="s">
+        <v>524</v>
+      </c>
+      <c r="E2" s="154" t="s">
+        <v>526</v>
+      </c>
+      <c r="F2" s="155" t="s">
+        <v>528</v>
+      </c>
+      <c r="G2" s="154" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+      <c r="A4" s="156" t="s">
+        <v>540</v>
+      </c>
+      <c r="B4" s="154" t="s">
+        <v>529</v>
+      </c>
+      <c r="C4" s="154" t="s">
+        <v>531</v>
+      </c>
+      <c r="D4" s="157" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A6" s="158" t="s">
+        <v>542</v>
+      </c>
+      <c r="B6" s="154" t="s">
+        <v>530</v>
+      </c>
+      <c r="C6" s="154" t="s">
+        <v>532</v>
+      </c>
+      <c r="D6" s="161" t="s">
+        <v>544</v>
+      </c>
+      <c r="G6" s="159" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A8" s="151" t="s">
+        <v>546</v>
+      </c>
+      <c r="B8" s="153" t="s">
+        <v>534</v>
+      </c>
+      <c r="D8" s="152" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+      <c r="B9" s="153" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="154" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+      <c r="B10" s="153" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="154" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="148" t="s">
+        <v>550</v>
+      </c>
+      <c r="C11" s="154" t="s">
+        <v>552</v>
+      </c>
+      <c r="D11" s="154" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="A13" s="151" t="s">
+        <v>537</v>
+      </c>
+      <c r="B13" s="153" t="s">
+        <v>553</v>
+      </c>
+      <c r="C13" s="154" t="s">
+        <v>538</v>
+      </c>
+      <c r="D13" s="150" t="s">
+        <v>554</v>
+      </c>
+      <c r="F13" s="155" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="A15" s="151" t="s">
+        <v>539</v>
+      </c>
+      <c r="B15" s="157" t="s">
+        <v>555</v>
+      </c>
+      <c r="C15" s="154" t="s">
+        <v>533</v>
+      </c>
+      <c r="F15" s="155" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="148" t="s">
+        <v>556</v>
+      </c>
+      <c r="C17" s="154" t="s">
+        <v>564</v>
+      </c>
+      <c r="D17" s="149" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="96" x14ac:dyDescent="0.2">
+      <c r="A19" s="148" t="s">
+        <v>558</v>
+      </c>
+      <c r="C19" s="154" t="s">
+        <v>565</v>
+      </c>
+      <c r="D19" s="160" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="148" t="s">
+        <v>560</v>
+      </c>
+      <c r="C21" s="154" t="s">
+        <v>566</v>
+      </c>
+      <c r="D21" s="149" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A23" s="148" t="s">
+        <v>562</v>
+      </c>
+      <c r="C23" s="154" t="s">
+        <v>567</v>
+      </c>
+      <c r="D23" s="149" t="s">
+        <v>563</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F13" r:id="rId2"/>
+    <hyperlink ref="F15" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -36157,7 +37027,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR15"/>
   <sheetViews>
@@ -36890,7 +37760,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H168"/>
   <sheetViews>
@@ -40721,7 +41591,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M220"/>
   <sheetViews>
@@ -47990,7 +48860,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AM18"/>
   <sheetViews>
@@ -48966,592 +49836,6 @@
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:AN20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="28" width="9.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="3:29" x14ac:dyDescent="0.2">
-      <c r="C1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E1" t="s">
-        <v>507</v>
-      </c>
-      <c r="G1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="2" spans="3:29" x14ac:dyDescent="0.2">
-      <c r="C2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="3:29" x14ac:dyDescent="0.2">
-      <c r="C3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="3:29" x14ac:dyDescent="0.2">
-      <c r="C6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="3:29" x14ac:dyDescent="0.2">
-      <c r="E7" s="24">
-        <v>41089</v>
-      </c>
-      <c r="F7" s="24">
-        <v>41180</v>
-      </c>
-      <c r="G7" s="24">
-        <v>41274</v>
-      </c>
-      <c r="H7" s="24">
-        <v>41361</v>
-      </c>
-      <c r="I7" s="24">
-        <v>41453</v>
-      </c>
-      <c r="J7" s="24">
-        <v>41547</v>
-      </c>
-      <c r="K7" s="24">
-        <v>41639</v>
-      </c>
-      <c r="L7" s="24">
-        <v>41729</v>
-      </c>
-      <c r="M7" s="24">
-        <v>41820</v>
-      </c>
-      <c r="N7" s="24">
-        <v>41912</v>
-      </c>
-      <c r="O7" s="24">
-        <v>42004</v>
-      </c>
-      <c r="P7" s="24">
-        <v>42094</v>
-      </c>
-      <c r="Q7" s="24">
-        <v>42185</v>
-      </c>
-      <c r="R7" s="24">
-        <v>42277</v>
-      </c>
-      <c r="S7" s="24">
-        <v>42369</v>
-      </c>
-      <c r="T7" s="24">
-        <v>42460</v>
-      </c>
-      <c r="U7" s="24">
-        <v>42551</v>
-      </c>
-      <c r="V7" s="24">
-        <v>42643</v>
-      </c>
-      <c r="W7" s="24">
-        <v>42734</v>
-      </c>
-      <c r="X7" s="24">
-        <v>42825</v>
-      </c>
-      <c r="Y7" s="24">
-        <v>42916</v>
-      </c>
-      <c r="Z7" s="24">
-        <v>43007</v>
-      </c>
-      <c r="AA7" s="24">
-        <v>43098</v>
-      </c>
-      <c r="AB7" s="24">
-        <v>43188</v>
-      </c>
-      <c r="AC7" s="90">
-        <v>43280</v>
-      </c>
-    </row>
-    <row r="8" spans="3:29" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8" t="s">
-        <v>56</v>
-      </c>
-      <c r="H8" t="s">
-        <v>56</v>
-      </c>
-      <c r="I8" t="s">
-        <v>56</v>
-      </c>
-      <c r="J8" t="s">
-        <v>56</v>
-      </c>
-      <c r="K8" t="s">
-        <v>56</v>
-      </c>
-      <c r="L8" t="s">
-        <v>56</v>
-      </c>
-      <c r="M8" t="s">
-        <v>56</v>
-      </c>
-      <c r="N8" t="s">
-        <v>56</v>
-      </c>
-      <c r="O8" t="s">
-        <v>56</v>
-      </c>
-      <c r="P8" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>56</v>
-      </c>
-      <c r="R8" t="s">
-        <v>56</v>
-      </c>
-      <c r="S8" t="s">
-        <v>56</v>
-      </c>
-      <c r="T8" t="s">
-        <v>56</v>
-      </c>
-      <c r="U8" t="s">
-        <v>56</v>
-      </c>
-      <c r="V8" t="s">
-        <v>56</v>
-      </c>
-      <c r="W8" t="s">
-        <v>56</v>
-      </c>
-      <c r="X8" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>56</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="3:29" x14ac:dyDescent="0.2">
-      <c r="C9" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="10" spans="3:29" x14ac:dyDescent="0.2">
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>289</v>
-      </c>
-      <c r="E10">
-        <v>150187</v>
-      </c>
-      <c r="F10">
-        <v>150544</v>
-      </c>
-      <c r="G10">
-        <v>150124</v>
-      </c>
-      <c r="H10">
-        <v>149395</v>
-      </c>
-      <c r="I10">
-        <v>148529</v>
-      </c>
-      <c r="J10">
-        <v>147610</v>
-      </c>
-      <c r="K10">
-        <v>145528</v>
-      </c>
-      <c r="L10">
-        <v>144686</v>
-      </c>
-      <c r="M10">
-        <v>144187</v>
-      </c>
-      <c r="N10">
-        <v>143354</v>
-      </c>
-      <c r="O10">
-        <v>140995</v>
-      </c>
-      <c r="P10">
-        <v>139206</v>
-      </c>
-      <c r="Q10">
-        <v>137303</v>
-      </c>
-      <c r="R10">
-        <v>137805</v>
-      </c>
-      <c r="S10">
-        <v>137504</v>
-      </c>
-      <c r="T10">
-        <v>137239</v>
-      </c>
-      <c r="U10">
-        <v>135874</v>
-      </c>
-      <c r="V10">
-        <v>133401</v>
-      </c>
-      <c r="W10">
-        <v>131501</v>
-      </c>
-      <c r="X10">
-        <v>128899</v>
-      </c>
-      <c r="Y10">
-        <v>127704</v>
-      </c>
-      <c r="Z10">
-        <v>125381</v>
-      </c>
-      <c r="AA10">
-        <v>123269</v>
-      </c>
-      <c r="AB10">
-        <v>121029</v>
-      </c>
-      <c r="AC10">
-        <v>118234</v>
-      </c>
-    </row>
-    <row r="11" spans="3:29" x14ac:dyDescent="0.2">
-      <c r="C11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" t="s">
-        <v>371</v>
-      </c>
-      <c r="E11">
-        <v>34719</v>
-      </c>
-      <c r="F11">
-        <v>36635</v>
-      </c>
-      <c r="G11">
-        <v>37878</v>
-      </c>
-      <c r="H11">
-        <v>39371</v>
-      </c>
-      <c r="I11">
-        <v>39948</v>
-      </c>
-      <c r="J11">
-        <v>40396</v>
-      </c>
-      <c r="K11">
-        <v>39250</v>
-      </c>
-      <c r="L11">
-        <v>39361</v>
-      </c>
-      <c r="M11">
-        <v>39669</v>
-      </c>
-      <c r="N11">
-        <v>38463</v>
-      </c>
-      <c r="O11">
-        <v>35583</v>
-      </c>
-      <c r="P11">
-        <v>33475</v>
-      </c>
-      <c r="Q11">
-        <v>31524</v>
-      </c>
-      <c r="R11">
-        <v>30212</v>
-      </c>
-      <c r="S11">
-        <v>28760</v>
-      </c>
-      <c r="T11">
-        <v>28716</v>
-      </c>
-      <c r="U11">
-        <v>27793</v>
-      </c>
-      <c r="V11">
-        <v>26737</v>
-      </c>
-      <c r="W11">
-        <v>25871</v>
-      </c>
-      <c r="X11">
-        <v>25175</v>
-      </c>
-      <c r="Y11">
-        <v>24450</v>
-      </c>
-      <c r="Z11">
-        <v>23779</v>
-      </c>
-      <c r="AA11">
-        <v>23282</v>
-      </c>
-      <c r="AB11">
-        <v>22545</v>
-      </c>
-      <c r="AC11" s="91">
-        <v>21317</v>
-      </c>
-    </row>
-    <row r="12" spans="3:29" x14ac:dyDescent="0.2">
-      <c r="C12">
-        <v>9</v>
-      </c>
-      <c r="D12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12">
-        <v>24879</v>
-      </c>
-      <c r="F12">
-        <v>27018</v>
-      </c>
-      <c r="G12">
-        <v>28366</v>
-      </c>
-      <c r="H12">
-        <v>29369</v>
-      </c>
-      <c r="I12">
-        <v>30326</v>
-      </c>
-      <c r="J12">
-        <v>31178</v>
-      </c>
-      <c r="K12">
-        <v>30706</v>
-      </c>
-      <c r="L12">
-        <v>31048</v>
-      </c>
-      <c r="M12">
-        <v>31749</v>
-      </c>
-      <c r="N12">
-        <v>31619</v>
-      </c>
-      <c r="O12">
-        <v>29224</v>
-      </c>
-      <c r="P12">
-        <v>27492</v>
-      </c>
-      <c r="Q12">
-        <v>26071</v>
-      </c>
-      <c r="R12">
-        <v>24809</v>
-      </c>
-      <c r="S12">
-        <v>23344</v>
-      </c>
-      <c r="T12">
-        <v>23270</v>
-      </c>
-      <c r="U12">
-        <v>22666</v>
-      </c>
-      <c r="V12">
-        <v>22095</v>
-      </c>
-      <c r="W12">
-        <v>21113</v>
-      </c>
-      <c r="X12">
-        <v>20601</v>
-      </c>
-      <c r="Y12">
-        <v>20191</v>
-      </c>
-      <c r="Z12">
-        <v>19405</v>
-      </c>
-      <c r="AA12">
-        <v>19018</v>
-      </c>
-      <c r="AB12">
-        <v>18363</v>
-      </c>
-      <c r="AC12">
-        <v>17394</v>
-      </c>
-    </row>
-    <row r="13" spans="3:29" x14ac:dyDescent="0.2">
-      <c r="C13">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E13">
-        <v>16.600000000000001</v>
-      </c>
-      <c r="F13">
-        <v>17.899999999999999</v>
-      </c>
-      <c r="G13">
-        <v>18.899999999999999</v>
-      </c>
-      <c r="H13">
-        <v>19.7</v>
-      </c>
-      <c r="I13">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="J13">
-        <v>21.1</v>
-      </c>
-      <c r="K13">
-        <v>21.1</v>
-      </c>
-      <c r="L13">
-        <v>21.5</v>
-      </c>
-      <c r="M13">
-        <v>22</v>
-      </c>
-      <c r="N13">
-        <v>22.1</v>
-      </c>
-      <c r="O13">
-        <v>20.7</v>
-      </c>
-      <c r="P13">
-        <v>19.7</v>
-      </c>
-      <c r="Q13">
-        <v>19</v>
-      </c>
-      <c r="R13">
-        <v>18</v>
-      </c>
-      <c r="S13">
-        <v>17</v>
-      </c>
-      <c r="T13">
-        <v>17</v>
-      </c>
-      <c r="U13">
-        <v>16.7</v>
-      </c>
-      <c r="V13">
-        <v>16.600000000000001</v>
-      </c>
-      <c r="W13">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="X13">
-        <v>16</v>
-      </c>
-      <c r="Y13">
-        <v>15.8</v>
-      </c>
-      <c r="Z13">
-        <v>15.5</v>
-      </c>
-      <c r="AA13">
-        <v>15.4</v>
-      </c>
-      <c r="AB13">
-        <v>15.2</v>
-      </c>
-      <c r="AC13">
-        <v>14.7</v>
-      </c>
-    </row>
-    <row r="20" spans="4:40" x14ac:dyDescent="0.2">
-      <c r="D20" s="25"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="26"/>
-      <c r="N20" s="27"/>
-      <c r="O20" s="26"/>
-      <c r="P20" s="27"/>
-      <c r="Q20" s="26"/>
-      <c r="R20" s="27"/>
-      <c r="S20" s="26"/>
-      <c r="T20" s="27"/>
-      <c r="U20" s="26"/>
-      <c r="V20" s="27"/>
-      <c r="W20" s="26"/>
-      <c r="X20" s="27"/>
-      <c r="Y20" s="26"/>
-      <c r="Z20" s="27"/>
-      <c r="AA20" s="26"/>
-      <c r="AB20" s="27"/>
-      <c r="AC20" s="26"/>
-      <c r="AD20" s="27"/>
-      <c r="AE20" s="26"/>
-      <c r="AF20" s="27"/>
-      <c r="AG20" s="26"/>
-      <c r="AH20" s="27"/>
-      <c r="AI20" s="26"/>
-      <c r="AJ20" s="27"/>
-      <c r="AK20" s="26"/>
-      <c r="AL20" s="27"/>
-      <c r="AM20" s="26"/>
-      <c r="AN20" s="31"/>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Start add Housing 2 fig 1 chart
</commit_message>
<xml_diff>
--- a/docs/housing_story_content/housing data story.xlsx
+++ b/docs/housing_story_content/housing data story.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1889" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1891" uniqueCount="570">
   <si>
     <t>Fingal</t>
   </si>
@@ -1812,6 +1812,12 @@
   </si>
   <si>
     <t>#traveller-accomodation-chart</t>
+  </si>
+  <si>
+    <t>House price index from 2005-2018 – national/Dublin housing/apartments</t>
+  </si>
+  <si>
+    <t>Tab 6, CSO</t>
   </si>
 </sst>
 </file>
@@ -3722,42 +3728,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3800,6 +3770,42 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="733">
@@ -4686,8 +4692,8 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="-1848856448"/>
-        <c:axId val="-1848854128"/>
+        <c:axId val="231279104"/>
+        <c:axId val="231281584"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -4763,11 +4769,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1848851296"/>
-        <c:axId val="-1848848976"/>
+        <c:axId val="231284576"/>
+        <c:axId val="231287056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1848856448"/>
+        <c:axId val="231279104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4794,7 +4800,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1848854128"/>
+        <c:crossAx val="231281584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4802,7 +4808,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1848854128"/>
+        <c:axId val="231281584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="8500.0"/>
@@ -4837,12 +4843,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1848856448"/>
+        <c:crossAx val="231279104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-1848851296"/>
+        <c:axId val="231284576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4851,7 +4857,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1848848976"/>
+        <c:crossAx val="231287056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4859,7 +4865,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1848848976"/>
+        <c:axId val="231287056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="18.0"/>
@@ -4888,7 +4894,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1848851296"/>
+        <c:crossAx val="231284576"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4942,7 +4948,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4986,7 +4992,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1100-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5030,7 +5036,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1100-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5074,7 +5080,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1100-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5118,7 +5124,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1100-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5167,7 +5173,7 @@
         <xdr:cNvPr id="2" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1500-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7324,13 +7330,13 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="141"/>
-      <c r="B5" s="141"/>
-      <c r="C5" s="141"/>
-      <c r="D5" s="141"/>
-      <c r="E5" s="141"/>
-      <c r="F5" s="141"/>
-      <c r="G5" s="141"/>
+      <c r="A5" s="156"/>
+      <c r="B5" s="156"/>
+      <c r="C5" s="156"/>
+      <c r="D5" s="156"/>
+      <c r="E5" s="156"/>
+      <c r="F5" s="156"/>
+      <c r="G5" s="156"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="44"/>
@@ -7381,15 +7387,15 @@
     <row r="10" spans="1:17" ht="39" x14ac:dyDescent="0.2">
       <c r="A10" s="45"/>
       <c r="B10" s="45"/>
-      <c r="C10" s="136"/>
-      <c r="D10" s="138"/>
+      <c r="C10" s="151"/>
+      <c r="D10" s="153"/>
       <c r="E10" s="56" t="s">
         <v>67</v>
       </c>
       <c r="F10" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="G10" s="140"/>
+      <c r="G10" s="155"/>
       <c r="J10" t="s">
         <v>400</v>
       </c>
@@ -7397,11 +7403,11 @@
     <row r="11" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="58"/>
       <c r="B11" s="58"/>
-      <c r="C11" s="137"/>
-      <c r="D11" s="139"/>
+      <c r="C11" s="152"/>
+      <c r="D11" s="154"/>
       <c r="E11" s="59"/>
       <c r="F11" s="60"/>
-      <c r="G11" s="140"/>
+      <c r="G11" s="155"/>
       <c r="K11" t="s">
         <v>401</v>
       </c>
@@ -11421,68 +11427,68 @@
     </row>
     <row r="3" spans="2:74" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="67"/>
-      <c r="C3" s="142" t="s">
+      <c r="C3" s="157" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="142"/>
-      <c r="E3" s="142"/>
-      <c r="F3" s="142"/>
-      <c r="G3" s="142"/>
-      <c r="H3" s="142"/>
-      <c r="I3" s="142"/>
-      <c r="J3" s="142"/>
-      <c r="K3" s="142"/>
-      <c r="L3" s="142"/>
-      <c r="M3" s="142"/>
-      <c r="N3" s="142"/>
-      <c r="O3" s="142"/>
-      <c r="P3" s="142"/>
-      <c r="Q3" s="142"/>
-      <c r="R3" s="142"/>
-      <c r="S3" s="142"/>
-      <c r="T3" s="142"/>
-      <c r="U3" s="142"/>
-      <c r="V3" s="142"/>
-      <c r="W3" s="142"/>
-      <c r="X3" s="142"/>
-      <c r="Y3" s="142"/>
-      <c r="Z3" s="142"/>
+      <c r="D3" s="157"/>
+      <c r="E3" s="157"/>
+      <c r="F3" s="157"/>
+      <c r="G3" s="157"/>
+      <c r="H3" s="157"/>
+      <c r="I3" s="157"/>
+      <c r="J3" s="157"/>
+      <c r="K3" s="157"/>
+      <c r="L3" s="157"/>
+      <c r="M3" s="157"/>
+      <c r="N3" s="157"/>
+      <c r="O3" s="157"/>
+      <c r="P3" s="157"/>
+      <c r="Q3" s="157"/>
+      <c r="R3" s="157"/>
+      <c r="S3" s="157"/>
+      <c r="T3" s="157"/>
+      <c r="U3" s="157"/>
+      <c r="V3" s="157"/>
+      <c r="W3" s="157"/>
+      <c r="X3" s="157"/>
+      <c r="Y3" s="157"/>
+      <c r="Z3" s="157"/>
     </row>
     <row r="4" spans="2:74" ht="16" x14ac:dyDescent="0.2">
-      <c r="B4" s="143" t="s">
+      <c r="B4" s="158" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="145" t="s">
+      <c r="C4" s="160" t="s">
         <v>73</v>
       </c>
-      <c r="D4" s="145"/>
-      <c r="E4" s="145"/>
-      <c r="F4" s="145"/>
-      <c r="G4" s="145"/>
-      <c r="H4" s="145"/>
-      <c r="I4" s="145"/>
-      <c r="J4" s="145"/>
-      <c r="K4" s="145"/>
-      <c r="L4" s="145"/>
-      <c r="M4" s="145"/>
-      <c r="N4" s="146"/>
-      <c r="O4" s="147" t="s">
+      <c r="D4" s="160"/>
+      <c r="E4" s="160"/>
+      <c r="F4" s="160"/>
+      <c r="G4" s="160"/>
+      <c r="H4" s="160"/>
+      <c r="I4" s="160"/>
+      <c r="J4" s="160"/>
+      <c r="K4" s="160"/>
+      <c r="L4" s="160"/>
+      <c r="M4" s="160"/>
+      <c r="N4" s="161"/>
+      <c r="O4" s="162" t="s">
         <v>74</v>
       </c>
-      <c r="P4" s="145"/>
-      <c r="Q4" s="145"/>
-      <c r="R4" s="145"/>
-      <c r="S4" s="145"/>
-      <c r="T4" s="145"/>
-      <c r="U4" s="145"/>
-      <c r="V4" s="145"/>
-      <c r="W4" s="145"/>
-      <c r="X4" s="145"/>
-      <c r="Y4" s="145"/>
-      <c r="Z4" s="146"/>
+      <c r="P4" s="160"/>
+      <c r="Q4" s="160"/>
+      <c r="R4" s="160"/>
+      <c r="S4" s="160"/>
+      <c r="T4" s="160"/>
+      <c r="U4" s="160"/>
+      <c r="V4" s="160"/>
+      <c r="W4" s="160"/>
+      <c r="X4" s="160"/>
+      <c r="Y4" s="160"/>
+      <c r="Z4" s="161"/>
     </row>
     <row r="5" spans="2:74" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="144"/>
+      <c r="B5" s="159"/>
       <c r="C5" s="68">
         <v>2002</v>
       </c>
@@ -36104,202 +36110,208 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.5" style="154" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" style="154" customWidth="1"/>
-    <col min="3" max="4" width="22.5" style="154" customWidth="1"/>
-    <col min="5" max="5" width="20.5" style="154" customWidth="1"/>
-    <col min="6" max="6" width="38.1640625" style="154" customWidth="1"/>
-    <col min="7" max="7" width="45" style="154" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="154"/>
+    <col min="1" max="1" width="43.5" style="142" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" style="142" customWidth="1"/>
+    <col min="3" max="4" width="22.5" style="142" customWidth="1"/>
+    <col min="5" max="5" width="20.5" style="142" customWidth="1"/>
+    <col min="6" max="6" width="38.1640625" style="142" customWidth="1"/>
+    <col min="7" max="7" width="45" style="142" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="142"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="150" t="s">
         <v>547</v>
       </c>
-      <c r="B1" s="162" t="s">
+      <c r="B1" s="150" t="s">
         <v>548</v>
       </c>
-      <c r="C1" s="162" t="s">
+      <c r="C1" s="150" t="s">
         <v>520</v>
       </c>
-      <c r="D1" s="162" t="s">
+      <c r="D1" s="150" t="s">
         <v>545</v>
       </c>
-      <c r="E1" s="162" t="s">
+      <c r="E1" s="150" t="s">
         <v>521</v>
       </c>
-      <c r="F1" s="162" t="s">
+      <c r="F1" s="150" t="s">
         <v>522</v>
       </c>
-      <c r="G1" s="154" t="s">
+      <c r="G1" s="142" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.2">
-      <c r="B2" s="154" t="s">
+      <c r="A2" s="142" t="s">
+        <v>568</v>
+      </c>
+      <c r="B2" s="142" t="s">
         <v>523</v>
       </c>
-      <c r="C2" s="154" t="s">
+      <c r="C2" s="142" t="s">
         <v>524</v>
       </c>
-      <c r="E2" s="154" t="s">
+      <c r="D2" s="137" t="s">
+        <v>569</v>
+      </c>
+      <c r="E2" s="142" t="s">
         <v>526</v>
       </c>
-      <c r="F2" s="155" t="s">
+      <c r="F2" s="143" t="s">
         <v>528</v>
       </c>
-      <c r="G2" s="154" t="s">
+      <c r="G2" s="142" t="s">
         <v>527</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A4" s="156" t="s">
+      <c r="A4" s="144" t="s">
         <v>540</v>
       </c>
-      <c r="B4" s="154" t="s">
+      <c r="B4" s="142" t="s">
         <v>529</v>
       </c>
-      <c r="C4" s="154" t="s">
+      <c r="C4" s="142" t="s">
         <v>531</v>
       </c>
-      <c r="D4" s="157" t="s">
+      <c r="D4" s="145" t="s">
         <v>541</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="158" t="s">
+      <c r="A6" s="146" t="s">
         <v>542</v>
       </c>
-      <c r="B6" s="154" t="s">
+      <c r="B6" s="142" t="s">
         <v>530</v>
       </c>
-      <c r="C6" s="154" t="s">
+      <c r="C6" s="142" t="s">
         <v>532</v>
       </c>
-      <c r="D6" s="161" t="s">
+      <c r="D6" s="149" t="s">
         <v>544</v>
       </c>
-      <c r="G6" s="159" t="s">
+      <c r="G6" s="147" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="A8" s="151" t="s">
+      <c r="A8" s="139" t="s">
         <v>546</v>
       </c>
-      <c r="B8" s="153" t="s">
+      <c r="B8" s="141" t="s">
         <v>534</v>
       </c>
-      <c r="D8" s="152" t="s">
+      <c r="D8" s="140" t="s">
         <v>549</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="B9" s="153" t="s">
+      <c r="B9" s="141" t="s">
         <v>89</v>
       </c>
-      <c r="C9" s="154" t="s">
+      <c r="C9" s="142" t="s">
         <v>535</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="B10" s="153" t="s">
+      <c r="B10" s="141" t="s">
         <v>90</v>
       </c>
-      <c r="C10" s="154" t="s">
+      <c r="C10" s="142" t="s">
         <v>536</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="148" t="s">
+      <c r="A11" s="136" t="s">
         <v>550</v>
       </c>
-      <c r="C11" s="154" t="s">
+      <c r="C11" s="142" t="s">
         <v>552</v>
       </c>
-      <c r="D11" s="154" t="s">
+      <c r="D11" s="142" t="s">
         <v>551</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.2">
-      <c r="A13" s="151" t="s">
+      <c r="A13" s="139" t="s">
         <v>537</v>
       </c>
-      <c r="B13" s="153" t="s">
+      <c r="B13" s="141" t="s">
         <v>553</v>
       </c>
-      <c r="C13" s="154" t="s">
+      <c r="C13" s="142" t="s">
         <v>538</v>
       </c>
-      <c r="D13" s="150" t="s">
+      <c r="D13" s="138" t="s">
         <v>554</v>
       </c>
-      <c r="F13" s="155" t="s">
+      <c r="F13" s="143" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.2">
-      <c r="A15" s="151" t="s">
+      <c r="A15" s="139" t="s">
         <v>539</v>
       </c>
-      <c r="B15" s="157" t="s">
+      <c r="B15" s="145" t="s">
         <v>555</v>
       </c>
-      <c r="C15" s="154" t="s">
+      <c r="C15" s="142" t="s">
         <v>533</v>
       </c>
-      <c r="F15" s="155" t="s">
+      <c r="F15" s="143" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="148" t="s">
+      <c r="A17" s="136" t="s">
         <v>556</v>
       </c>
-      <c r="C17" s="154" t="s">
+      <c r="C17" s="142" t="s">
         <v>564</v>
       </c>
-      <c r="D17" s="149" t="s">
+      <c r="D17" s="137" t="s">
         <v>557</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="96" x14ac:dyDescent="0.2">
-      <c r="A19" s="148" t="s">
+      <c r="A19" s="136" t="s">
         <v>558</v>
       </c>
-      <c r="C19" s="154" t="s">
+      <c r="C19" s="142" t="s">
         <v>565</v>
       </c>
-      <c r="D19" s="160" t="s">
+      <c r="D19" s="148" t="s">
         <v>559</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="148" t="s">
+      <c r="A21" s="136" t="s">
         <v>560</v>
       </c>
-      <c r="C21" s="154" t="s">
+      <c r="C21" s="142" t="s">
         <v>566</v>
       </c>
-      <c r="D21" s="149" t="s">
+      <c r="D21" s="137" t="s">
         <v>561</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A23" s="148" t="s">
+      <c r="A23" s="136" t="s">
         <v>562</v>
       </c>
-      <c r="C23" s="154" t="s">
+      <c r="C23" s="142" t="s">
         <v>567</v>
       </c>
-      <c r="D23" s="149" t="s">
+      <c r="D23" s="137" t="s">
         <v>563</v>
       </c>
     </row>

</xml_diff>